<commit_message>
Change distance dependency function
</commit_message>
<xml_diff>
--- a/media/toa-do.xlsx
+++ b/media/toa-do.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Map 01" sheetId="1" state="visible" r:id="rId2"/>
@@ -2286,7 +2286,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2337,8 +2337,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2368,10 +2368,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>1420</v>
+        <v>1450</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>890</v>
+        <v>850</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>90</v>
@@ -2385,10 +2385,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>3120</v>
+        <v>3140</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1190</v>
+        <v>1200</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>90</v>

</xml_diff>

<commit_message>
Update fuzzy_dependency function and traffic lamp coordinate
</commit_message>
<xml_diff>
--- a/media/toa-do.xlsx
+++ b/media/toa-do.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Map 01" sheetId="1" state="visible" r:id="rId2"/>
@@ -2337,7 +2337,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2493,8 +2493,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2524,10 +2524,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1610</v>
+        <v>1630</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>90</v>

</xml_diff>